<commit_message>
Minor update for eeprom.
</commit_message>
<xml_diff>
--- a/EEPROMMap.xlsx
+++ b/EEPROMMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Page 0 EEPROM Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="113">
   <si>
-    <t xml:space="preserve">Page 0 Add \ byte</t>
+    <t xml:space="preserve">Page 0 Address \ byte</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -563,13 +563,13 @@
   </sheetPr>
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="2" style="2" width="6.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
   </cols>
@@ -1845,8 +1845,8 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1960,106 +1960,106 @@
       <c r="A9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
       <c r="D18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="18"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
       <c r="D21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Minor change for EEPROMMap.xlsx
</commit_message>
<xml_diff>
--- a/EEPROMMap.xlsx
+++ b/EEPROMMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Page 0 EEPROM Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,9 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="113">
-  <si>
-    <t xml:space="preserve">Page 0 Address \ byte</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
+  <si>
+    <t xml:space="preserve">Page 0 Address \ Byte</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -192,7 +192,7 @@
     <t xml:space="preserve">95# Encryption</t>
   </si>
   <si>
-    <t xml:space="preserve">Page 1 Add \ byte</t>
+    <t xml:space="preserve">Page 1 Address \ Byte</t>
   </si>
   <si>
     <t xml:space="preserve">41#</t>
@@ -297,18 +297,27 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">Used?</t>
+  </si>
+  <si>
     <t xml:space="preserve">'P’ or ‘S’</t>
   </si>
   <si>
     <t xml:space="preserve">Pending/Sending</t>
   </si>
   <si>
+    <t xml:space="preserve">v</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x01</t>
   </si>
   <si>
     <t xml:space="preserve">Dial Type</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">0xF2</t>
   </si>
   <si>
@@ -325,6 +334,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reboot Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">???</t>
   </si>
   <si>
     <t xml:space="preserve">MM Count</t>
@@ -370,7 +382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -394,6 +406,12 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -459,7 +477,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -492,7 +510,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,12 +558,24 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -553,6 +587,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -563,8 +657,8 @@
   </sheetPr>
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -771,24 +865,24 @@
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
@@ -873,19 +967,19 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
@@ -894,309 +988,309 @@
       <c r="B12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-    </row>
-    <row r="27" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10"/>
-      <c r="B27" s="9" t="s">
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+    </row>
+    <row r="27" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11"/>
+      <c r="B27" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -1248,12 +1342,12 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="2" style="2" width="6.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
   </cols>
@@ -1692,39 +1786,39 @@
       <c r="I13" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
@@ -1757,44 +1851,44 @@
         <v>85</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -1843,463 +1937,552 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="27.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="39.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="27.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="39.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>90</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="18"/>
+      <c r="C2" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="18"/>
+      <c r="B4" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="n">
+      <c r="B7" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="18"/>
+      <c r="C7" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="n">
+      <c r="B8" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="18"/>
+      <c r="C8" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="18"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="21" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="18"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="18"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="18"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="18"/>
+      <c r="B22" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="19"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
+      <c r="B23" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="19" t="n">
+      <c r="B24" s="22" t="n">
         <v>7548</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>103</v>
+      <c r="C24" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="20"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="20"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="19" t="n">
+      <c r="B29" s="22" t="n">
         <v>4007</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>106</v>
+      <c r="C29" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="20"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="20"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="20"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="18"/>
+      <c r="B33" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="21" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="21"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="21"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="21"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="18"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="21"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="21"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="18"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="21"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="18"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="21"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="18"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="21"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="18"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="19"/>
+      <c r="E42" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" s="18"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="19"/>
+      <c r="E43" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="18"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="E44" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="B45" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D45" s="18"/>
+      <c r="B45" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="E45" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
     <mergeCell ref="B9:C21"/>
     <mergeCell ref="D9:D21"/>
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="E9:E21"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
     <mergeCell ref="B29:B32"/>
     <mergeCell ref="C29:C32"/>
     <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E29:E32"/>
     <mergeCell ref="B33:B41"/>
     <mergeCell ref="C33:C41"/>
     <mergeCell ref="D33:D41"/>
+    <mergeCell ref="E33:E41"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Updated RF device ID only allows 16 entries 41 ~ 56
</commit_message>
<xml_diff>
--- a/EEPROMMap.xlsx
+++ b/EEPROMMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Page 0 EEPROM Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="111">
   <si>
     <t xml:space="preserve">Add \ Byte</t>
   </si>
@@ -252,34 +252,19 @@
     <t xml:space="preserve">0x80</t>
   </si>
   <si>
-    <t xml:space="preserve">57#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61#</t>
-  </si>
-  <si>
     <t xml:space="preserve">62#</t>
   </si>
   <si>
-    <t xml:space="preserve">63#</t>
-  </si>
-  <si>
     <t xml:space="preserve">36# OTA IP</t>
   </si>
   <si>
+    <t xml:space="preserve">0xF0</t>
+  </si>
+  <si>
     <t xml:space="preserve">37# OTA Port</t>
   </si>
   <si>
-    <t xml:space="preserve">41# ~ 63# RF Device ID</t>
+    <t xml:space="preserve">41# ~ 56# RF Device ID</t>
   </si>
   <si>
     <t xml:space="preserve">stack_buffer BYTE</t>
@@ -384,6 +369,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -405,12 +391,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -515,7 +503,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -646,13 +634,13 @@
   </sheetPr>
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="2" style="2" width="6.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
   </cols>
@@ -911,8 +899,10 @@
       <c r="O9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
+      <c r="P9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
@@ -1282,7 +1272,7 @@
       <c r="Q29" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:Q3"/>
     <mergeCell ref="B4:Q4"/>
@@ -1294,6 +1284,7 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:I9"/>
+    <mergeCell ref="P9:Q9"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="L10:Q10"/>
     <mergeCell ref="B11:F11"/>
@@ -1331,12 +1322,12 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="2" style="2" width="6.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
   </cols>
@@ -1662,98 +1653,78 @@
       <c r="A10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="B10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="6" t="n">
+      <c r="B12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1761,23 +1732,17 @@
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
@@ -1814,7 +1779,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1837,29 +1802,52 @@
         <v>41</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>44</v>
@@ -1880,7 +1868,7 @@
       <c r="Q20" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="26">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="B3:G3"/>
@@ -1897,23 +1885,20 @@
     <mergeCell ref="J8:O8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="J9:O9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="J13:Q13"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="B13:Q13"/>
     <mergeCell ref="B14:Q14"/>
     <mergeCell ref="B15:Q15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:Q16"/>
+    <mergeCell ref="B16:Q16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:Q17"/>
     <mergeCell ref="B20:Q20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05416666666667" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1928,35 +1913,35 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="27.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="39.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="39.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,14 +1949,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,14 +1964,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,14 +1979,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,14 +1994,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,14 +2009,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,13 +2027,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,13 +2044,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,7 +2063,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="19"/>
       <c r="E9" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,7 +2182,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="6"/>
@@ -2221,13 +2206,13 @@
         <v>7548</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2262,12 +2247,12 @@
         <v>26</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="19"/>
       <c r="E28" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,13 +2263,13 @@
         <v>4007</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,14 +2304,14 @@
         <v>31</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,11 +2392,11 @@
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,11 +2405,11 @@
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,11 +2418,11 @@
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,14 +2430,14 @@
         <v>43</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2477,7 +2462,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05416666666667" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Changed stack_buffer size to 50.
</commit_message>
<xml_diff>
--- a/EEPROMMap.xlsx
+++ b/EEPROMMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Page 0 EEPROM Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="117">
   <si>
     <t xml:space="preserve">Add \ Byte</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t xml:space="preserve">16#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not used</t>
   </si>
   <si>
     <t xml:space="preserve">0xC0</t>
@@ -646,8 +649,8 @@
   </sheetPr>
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -911,15 +914,17 @@
       <c r="O9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
+      <c r="P9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -928,16 +933,16 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -947,10 +952,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -972,10 +977,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>21</v>
@@ -997,10 +1002,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -1019,10 +1024,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -1041,10 +1046,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -1063,10 +1068,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -1085,10 +1090,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -1107,10 +1112,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -1129,10 +1134,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -1151,10 +1156,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1173,10 +1178,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -1195,10 +1200,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -1218,7 +1223,7 @@
     <row r="27" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
       <c r="B27" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1239,10 +1244,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -1261,10 +1266,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -1282,7 +1287,7 @@
       <c r="Q29" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:Q3"/>
     <mergeCell ref="B4:Q4"/>
@@ -1294,6 +1299,7 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:I9"/>
+    <mergeCell ref="P9:Q9"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="L10:Q10"/>
     <mergeCell ref="B11:F11"/>
@@ -1399,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1413,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1432,7 +1438,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1446,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -1462,10 +1468,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1479,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -1498,7 +1504,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1512,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -1528,10 +1534,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1545,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -1564,7 +1570,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1578,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1594,10 +1600,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1611,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1630,7 +1636,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1644,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -1660,10 +1666,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1677,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1696,7 +1702,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1710,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -1729,7 +1735,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1743,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1762,7 +1768,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1788,7 +1794,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>21</v>
@@ -1811,10 +1817,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1834,10 +1840,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="8" t="s">
@@ -1859,10 +1865,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -1928,7 +1934,7 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -1944,19 +1950,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,14 +1970,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,14 +1985,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,14 +2000,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,14 +2015,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,14 +2030,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,13 +2048,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,13 +2065,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,7 +2084,7 @@
       <c r="C9" s="20"/>
       <c r="D9" s="19"/>
       <c r="E9" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,7 +2203,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="6"/>
@@ -2221,13 +2227,13 @@
         <v>7548</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2262,12 +2268,12 @@
         <v>26</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="19"/>
       <c r="E28" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,13 +2284,13 @@
         <v>4007</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,14 +2325,14 @@
         <v>31</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,11 +2413,11 @@
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="18" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,11 +2426,11 @@
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,11 +2439,11 @@
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,14 +2451,14 @@
         <v>43</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check in page0_eeprom/page1_eeprom struct code. Should be always keep updated EEPROM info as global varialbe. Changes - Added FR (first run) in page 0 address 0x04. The function is not working yet. - Added init_pic18_eeprom() to replace init_eeprom().
</commit_message>
<xml_diff>
--- a/EEPROMMap.xlsx
+++ b/EEPROMMap.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="122">
   <si>
     <t xml:space="preserve">Add \ Byte</t>
   </si>
@@ -51,6 +51,9 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
+    <t xml:space="preserve">FR</t>
+  </si>
+  <si>
     <t xml:space="preserve">reserved1</t>
   </si>
   <si>
@@ -168,18 +171,39 @@
     <t xml:space="preserve">08#</t>
   </si>
   <si>
+    <t xml:space="preserve">reserved8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xD0</t>
+  </si>
+  <si>
     <t xml:space="preserve">10# Unit Account</t>
   </si>
   <si>
-    <t xml:space="preserve">0xD0</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reserved8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">11# Line Card</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">11# Line Card</t>
   </si>
   <si>
-    <t xml:space="preserve">reserved8</t>
-  </si>
-  <si>
     <t xml:space="preserve">0xE0</t>
   </si>
   <si>
@@ -190,6 +214,9 @@
   </si>
   <si>
     <t xml:space="preserve">0xF0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR First Run – used to check if we need init EEPROM</t>
   </si>
   <si>
     <t xml:space="preserve">MM Count -  used for data sequence</t>
@@ -388,7 +415,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -422,11 +449,16 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -498,7 +530,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -531,7 +563,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,7 +571,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -547,6 +579,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -563,7 +599,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -680,10 +716,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -756,10 +792,12 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
@@ -770,15 +808,15 @@
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -798,10 +836,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -821,10 +859,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -844,10 +882,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -867,10 +905,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -890,33 +928,33 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -936,33 +974,33 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
+      <c r="B10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -982,76 +1020,76 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="B12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" s="6"/>
+      <c r="P13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1060,40 +1098,42 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="L14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="G15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -1104,59 +1144,57 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>57</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -1173,273 +1211,295 @@
       <c r="Q21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
+      <c r="B22" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
+      <c r="B23" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
+      <c r="B25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
+      <c r="B26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
+      <c r="B27" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
+      <c r="B28" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+    </row>
+    <row r="32" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14"/>
+      <c r="B32" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-    </row>
-    <row r="31" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13"/>
-      <c r="B31" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="13"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
+      <c r="C33" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="37">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:P2"/>
+    <mergeCell ref="G2:P2"/>
     <mergeCell ref="B3:Q3"/>
     <mergeCell ref="B4:Q4"/>
     <mergeCell ref="B5:Q5"/>
@@ -1457,8 +1517,8 @@
     <mergeCell ref="P13:Q13"/>
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="L14:Q14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="G15:Q15"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="J15:Q15"/>
     <mergeCell ref="C16:Q16"/>
     <mergeCell ref="B17:Q17"/>
     <mergeCell ref="B21:Q21"/>
@@ -1474,6 +1534,7 @@
     <mergeCell ref="B31:Q31"/>
     <mergeCell ref="B32:Q32"/>
     <mergeCell ref="B33:Q33"/>
+    <mergeCell ref="B34:Q34"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05416666666667" header="0.7875" footer="0.7875"/>
@@ -1492,7 +1553,7 @@
   </sheetPr>
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1561,7 +1622,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1575,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1591,10 +1652,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1608,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -1624,10 +1685,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1641,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -1657,10 +1718,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1674,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -1690,10 +1751,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1707,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -1723,10 +1784,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1740,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1756,10 +1817,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1773,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1789,10 +1850,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1806,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -1822,117 +1883,117 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
+        <v>28</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
+        <v>32</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1952,73 +2013,73 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="D17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
+      <c r="B20" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -2062,531 +2123,531 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="18" width="27.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="19" width="39.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="27.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>93</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="23"/>
+      <c r="B2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="24"/>
       <c r="E2" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="23"/>
+      <c r="B3" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="24"/>
       <c r="E3" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="23"/>
+      <c r="B4" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="24"/>
       <c r="E4" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="21" t="n">
+      <c r="B7" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>106</v>
+      <c r="C7" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="21" t="n">
+      <c r="B8" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>106</v>
+      <c r="C8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="23"/>
+      <c r="B9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="23"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="23"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="23"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="23"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="23"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="23"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="23"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="23"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="23"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="23"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D22" s="23"/>
+      <c r="B22" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="24"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
+      <c r="B23" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="24" t="n">
+      <c r="B24" s="25" t="n">
         <v>7548</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>96</v>
+      <c r="C24" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="25"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
+      <c r="B28" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
       <c r="E28" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="24" t="n">
+      <c r="B29" s="25" t="n">
         <v>4007</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>112</v>
+      <c r="C29" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>115</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="26"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="26"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="B33" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" s="23"/>
+      <c r="B33" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="24"/>
       <c r="E33" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="23"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
       <c r="E34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="24"/>
       <c r="E35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="23"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
       <c r="E36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="23"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
       <c r="E37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="23"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="23"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24"/>
       <c r="E39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="23"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="23"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
       <c r="E41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="23"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="24"/>
       <c r="E42" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" s="23"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="24"/>
       <c r="E43" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="23"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="24"/>
       <c r="E44" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="B45" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D45" s="23"/>
+      <c r="B45" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="24"/>
       <c r="E45" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified stack_buffer to be a union of uint8_t array and emc_t struct.
</commit_message>
<xml_diff>
--- a/EEPROMMap.xlsx
+++ b/EEPROMMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Page 0 EEPROM Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
   <si>
     <t xml:space="preserve">Add \ Byte</t>
   </si>
@@ -180,25 +180,7 @@
     <t xml:space="preserve">10# Unit Account</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">reserved8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">11# Line Card</t>
-    </r>
+    <t xml:space="preserve">reserved8 11# Line Card</t>
   </si>
   <si>
     <t xml:space="preserve">11# Line Card</t>
@@ -318,7 +300,10 @@
     <t xml:space="preserve">41# ~ 56# RF Device ID (ONLY 16 ID now)</t>
   </si>
   <si>
-    <t xml:space="preserve">stack_buffer BYTE</t>
+    <t xml:space="preserve">stack_buffer OFFSET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">length</t>
   </si>
   <si>
     <t xml:space="preserve">value</t>
@@ -333,12 +318,15 @@
     <t xml:space="preserve">Used?</t>
   </si>
   <si>
-    <t xml:space="preserve">'P’ or ‘S’</t>
+    <t xml:space="preserve">'P’ / ‘S’ / ‘T’</t>
   </si>
   <si>
     <t xml:space="preserve">Pending/Sending</t>
   </si>
   <si>
+    <t xml:space="preserve">'P' - pending, 'S' - sending, 'T' - ???</t>
+  </si>
+  <si>
     <t xml:space="preserve">v</t>
   </si>
   <si>
@@ -372,22 +360,22 @@
     <t xml:space="preserve">???</t>
   </si>
   <si>
+    <t xml:space="preserve">13 bytes</t>
+  </si>
+  <si>
     <t xml:space="preserve">MM Count</t>
   </si>
   <si>
     <t xml:space="preserve">Line Card</t>
   </si>
   <si>
-    <t xml:space="preserve">Max 4 bytes (See Page 0 EEPROM struct)</t>
+    <t xml:space="preserve">Max 8 bytes (See Page 0 EEPROM struct) ???</t>
   </si>
   <si>
     <t xml:space="preserve">',’</t>
   </si>
   <si>
     <t xml:space="preserve">Unit Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max 5 bytes (See Page 0 EEPROM struct)</t>
   </si>
   <si>
     <t xml:space="preserve">"18,115400"</t>
@@ -415,12 +403,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -439,14 +426,84 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFC9211E"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -455,20 +512,56 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFC9211E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -489,12 +582,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -505,7 +613,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -529,13 +637,64 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -543,39 +702,35 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,12 +750,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -615,53 +766,74 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -673,7 +845,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -689,7 +861,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -718,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1022,24 +1194,24 @@
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
@@ -1079,10 +1251,10 @@
       <c r="O13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="P13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="Q13" s="9"/>
+      <c r="Q13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
@@ -1106,14 +1278,14 @@
       <c r="K14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="L14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
@@ -1131,41 +1303,41 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
@@ -1191,310 +1363,310 @@
       <c r="Q17" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-    </row>
-    <row r="32" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14"/>
-      <c r="B32" s="13" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+    </row>
+    <row r="32" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13"/>
+      <c r="B32" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="14"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -1554,7 +1726,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1885,108 +2057,108 @@
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
@@ -2015,24 +2187,24 @@
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
@@ -2042,44 +2214,44 @@
         <v>90</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -2121,554 +2293,643 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="27.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="39.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="27.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="39.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>96</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="21" t="s">
         <v>99</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="5" t="s">
+      <c r="B3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>102</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="23" t="s">
+      <c r="B4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="5" t="s">
-        <v>102</v>
+      <c r="B5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="23" t="s">
+      <c r="B6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="5" t="s">
-        <v>102</v>
+      <c r="D6" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="22" t="n">
+      <c r="B7" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>99</v>
+      <c r="D7" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="22" t="n">
+      <c r="B8" s="23"/>
+      <c r="C8" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>99</v>
+      <c r="D8" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="23" t="n">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="7" t="s">
-        <v>102</v>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="7"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="7"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="7"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="7"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="7"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="7"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="7"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="7"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="23"/>
+      <c r="C23" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="5"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="25" t="n">
+      <c r="B24" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" s="25" t="n">
         <v>7548</v>
       </c>
-      <c r="C24" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>99</v>
+      <c r="D24" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="25"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="25"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="25"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="25"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="25"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="25"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="5" t="s">
-        <v>99</v>
+      <c r="B28" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="25" t="n">
+      <c r="B29" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="25" t="n">
         <v>4007</v>
       </c>
-      <c r="C29" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>99</v>
+      <c r="F29" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="5"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="5"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="5"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="B33" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="7" t="s">
-        <v>99</v>
+      <c r="B33" s="23" t="n">
+        <v>9</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="24"/>
+      <c r="F33" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="7"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="7"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="7"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="7"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="7"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="7"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="7"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="7"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="22"/>
-      <c r="C42" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" s="24"/>
-      <c r="E42" s="5" t="s">
-        <v>99</v>
+      <c r="B42" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="22"/>
+      <c r="F42" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
         <v>41</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="24"/>
-      <c r="E43" s="5" t="s">
-        <v>99</v>
+      <c r="B43" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="22"/>
+      <c r="F43" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" s="24"/>
-      <c r="E44" s="5" t="s">
-        <v>99</v>
+      <c r="B44" s="23"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="22"/>
+      <c r="F44" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
         <v>43</v>
       </c>
-      <c r="B45" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="D45" s="24"/>
-      <c r="E45" s="5" t="s">
-        <v>99</v>
+      <c r="B45" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B9:C21"/>
-    <mergeCell ref="D9:D21"/>
+  <mergeCells count="24">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B21"/>
+    <mergeCell ref="C9:D21"/>
     <mergeCell ref="E9:E21"/>
-    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="F9:F21"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
     <mergeCell ref="B29:B32"/>
     <mergeCell ref="C29:C32"/>
     <mergeCell ref="D29:D32"/>
     <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F29:F32"/>
     <mergeCell ref="B33:B41"/>
     <mergeCell ref="C33:C41"/>
     <mergeCell ref="D33:D41"/>
     <mergeCell ref="E33:E41"/>
+    <mergeCell ref="F33:F41"/>
+    <mergeCell ref="B43:B44"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05416666666667" header="0.7875" footer="0.7875"/>

</xml_diff>